<commit_message>
Popular car model implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="BikeDetails" r:id="rId3" sheetId="1"/>
+    <sheet name="PopularCarModels" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Bike Name</t>
   </si>
@@ -81,6 +82,36 @@
   </si>
   <si>
     <t>Honda Rebel 300</t>
+  </si>
+  <si>
+    <t>Popular Car Model</t>
+  </si>
+  <si>
+    <t>Maruti 800</t>
+  </si>
+  <si>
+    <t>Maruti Swift Dzire</t>
+  </si>
+  <si>
+    <t>Maruti Swift</t>
+  </si>
+  <si>
+    <t>Hyundai I10</t>
+  </si>
+  <si>
+    <t>Hyundai Santro Xing</t>
+  </si>
+  <si>
+    <t>Honda City</t>
+  </si>
+  <si>
+    <t>Toyota Innova</t>
+  </si>
+  <si>
+    <t>Toyota Fortuner</t>
+  </si>
+  <si>
+    <t>Mahindra XUV500</t>
   </si>
 </sst>
 </file>
@@ -88,13 +119,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -142,11 +178,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -266,4 +303,70 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.171875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Upcoming Tata car details implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="BikeDetails" r:id="rId3" sheetId="1"/>
     <sheet name="PopularCarModels" r:id="rId4" sheetId="2"/>
+    <sheet name="CarDetails" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Bike Name</t>
   </si>
@@ -112,6 +113,102 @@
   </si>
   <si>
     <t>Mahindra XUV500</t>
+  </si>
+  <si>
+    <t>Car Name</t>
+  </si>
+  <si>
+    <t>Car Price</t>
+  </si>
+  <si>
+    <t>Tata Altroz Racer</t>
+  </si>
+  <si>
+    <t>Rs. 10.00 Lakh</t>
+  </si>
+  <si>
+    <t>20 Mar 2024</t>
+  </si>
+  <si>
+    <t>Tata Curvv EV</t>
+  </si>
+  <si>
+    <t>Rs. 20.00 Lakh</t>
+  </si>
+  <si>
+    <t>Jul 2024</t>
+  </si>
+  <si>
+    <t>Tata Curvv</t>
+  </si>
+  <si>
+    <t>Rs. 10.50 Lakh</t>
+  </si>
+  <si>
+    <t>Aug 2024</t>
+  </si>
+  <si>
+    <t>Tata Avinya</t>
+  </si>
+  <si>
+    <t>Rs. 30.00 Lakh</t>
+  </si>
+  <si>
+    <t>Jan 2025</t>
+  </si>
+  <si>
+    <t>Tata Harrier EV</t>
+  </si>
+  <si>
+    <t>Apr 2025</t>
+  </si>
+  <si>
+    <t>Tata Punch 2025</t>
+  </si>
+  <si>
+    <t>Rs. 6.00 Lakh</t>
+  </si>
+  <si>
+    <t>Jun 2025</t>
+  </si>
+  <si>
+    <t>Tata Sierra</t>
+  </si>
+  <si>
+    <t>Rs. 25.00 Lakh</t>
+  </si>
+  <si>
+    <t>Dec 2025</t>
+  </si>
+  <si>
+    <t>Tata Kite 5</t>
+  </si>
+  <si>
+    <t>Rs. 4.50 Lakh</t>
+  </si>
+  <si>
+    <t>Tata Atmos</t>
+  </si>
+  <si>
+    <t>Rs. 12.00 Lakh</t>
+  </si>
+  <si>
+    <t>Tata H7X</t>
+  </si>
+  <si>
+    <t>Rs. 15.00 Lakh</t>
+  </si>
+  <si>
+    <t>Tata Altroz EV</t>
+  </si>
+  <si>
+    <t>Rs. 14.00 Lakh</t>
+  </si>
+  <si>
+    <t>Tata Hexa</t>
+  </si>
+  <si>
+    <t>Tata EVision Electric</t>
   </si>
 </sst>
 </file>
@@ -119,13 +216,28 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -178,12 +290,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -369,4 +484,176 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.0390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.37109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.140625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cucumber and extent report implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -15,7 +15,202 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="97">
+  <si>
+    <t>Bike Name</t>
+  </si>
+  <si>
+    <t>Bike Price</t>
+  </si>
+  <si>
+    <t>Launch Date</t>
+  </si>
+  <si>
+    <t>Honda CRF300L</t>
+  </si>
+  <si>
+    <t>Rs. 3.30 Lakh</t>
+  </si>
+  <si>
+    <t>30 Mar 2024</t>
+  </si>
+  <si>
+    <t>Honda Activa Electric</t>
+  </si>
+  <si>
+    <t>Rs. 1.10 Lakh</t>
+  </si>
+  <si>
+    <t>Mar 2024</t>
+  </si>
+  <si>
+    <t>Honda Forza 350</t>
+  </si>
+  <si>
+    <t>Rs. 3.70 Lakh</t>
+  </si>
+  <si>
+    <t>Honda CB350 Cruiser</t>
+  </si>
+  <si>
+    <t>Rs. 2.30 Lakh</t>
+  </si>
+  <si>
+    <t>Honda Activa 7G</t>
+  </si>
+  <si>
+    <t>Rs. 79,000</t>
+  </si>
+  <si>
+    <t>Apr 2024</t>
+  </si>
+  <si>
+    <t>Honda PCX160</t>
+  </si>
+  <si>
+    <t>Rs. 1.20 Lakh</t>
+  </si>
+  <si>
+    <t>Jun 2024</t>
+  </si>
+  <si>
+    <t>Honda CBR150R</t>
+  </si>
+  <si>
+    <t>Rs. 1.70 Lakh</t>
+  </si>
+  <si>
+    <t>Unrevealed</t>
+  </si>
+  <si>
+    <t>Honda Rebel 300</t>
+  </si>
+  <si>
+    <t>Popular Car Model</t>
+  </si>
+  <si>
+    <t>Maruti 800</t>
+  </si>
+  <si>
+    <t>Maruti Swift Dzire</t>
+  </si>
+  <si>
+    <t>Maruti Swift</t>
+  </si>
+  <si>
+    <t>Hyundai I10</t>
+  </si>
+  <si>
+    <t>Hyundai Santro Xing</t>
+  </si>
+  <si>
+    <t>Honda City</t>
+  </si>
+  <si>
+    <t>Toyota Innova</t>
+  </si>
+  <si>
+    <t>Toyota Fortuner</t>
+  </si>
+  <si>
+    <t>Mahindra XUV500</t>
+  </si>
+  <si>
+    <t>Car Name</t>
+  </si>
+  <si>
+    <t>Car Price</t>
+  </si>
+  <si>
+    <t>Tata Altroz Racer</t>
+  </si>
+  <si>
+    <t>Rs. 10.00 Lakh</t>
+  </si>
+  <si>
+    <t>20 Mar 2024</t>
+  </si>
+  <si>
+    <t>Tata Curvv EV</t>
+  </si>
+  <si>
+    <t>Rs. 20.00 Lakh</t>
+  </si>
+  <si>
+    <t>Jul 2024</t>
+  </si>
+  <si>
+    <t>Tata Curvv</t>
+  </si>
+  <si>
+    <t>Rs. 10.50 Lakh</t>
+  </si>
+  <si>
+    <t>Aug 2024</t>
+  </si>
+  <si>
+    <t>Tata Avinya</t>
+  </si>
+  <si>
+    <t>Rs. 30.00 Lakh</t>
+  </si>
+  <si>
+    <t>Jan 2025</t>
+  </si>
+  <si>
+    <t>Tata Harrier EV</t>
+  </si>
+  <si>
+    <t>Apr 2025</t>
+  </si>
+  <si>
+    <t>Tata Punch 2025</t>
+  </si>
+  <si>
+    <t>Rs. 6.00 Lakh</t>
+  </si>
+  <si>
+    <t>Jun 2025</t>
+  </si>
+  <si>
+    <t>Tata Sierra</t>
+  </si>
+  <si>
+    <t>Rs. 25.00 Lakh</t>
+  </si>
+  <si>
+    <t>Dec 2025</t>
+  </si>
+  <si>
+    <t>Tata Kite 5</t>
+  </si>
+  <si>
+    <t>Rs. 4.50 Lakh</t>
+  </si>
+  <si>
+    <t>Tata Atmos</t>
+  </si>
+  <si>
+    <t>Rs. 12.00 Lakh</t>
+  </si>
+  <si>
+    <t>Tata H7X</t>
+  </si>
+  <si>
+    <t>Rs. 15.00 Lakh</t>
+  </si>
+  <si>
+    <t>Tata Altroz EV</t>
+  </si>
+  <si>
+    <t>Rs. 14.00 Lakh</t>
+  </si>
+  <si>
+    <t>Tata Hexa</t>
+  </si>
+  <si>
+    <t>Tata EVision Electric</t>
+  </si>
   <si>
     <t>Health Insurance Brand Name</t>
   </si>
@@ -133,13 +328,48 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -182,23 +412,133 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.90625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.37109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.140625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -206,13 +546,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.171875" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="s" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -220,13 +612,171 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.0390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.37109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.140625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -245,131 +795,131 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="2">
-        <v>16</v>
+      <c r="A1" t="s" s="8">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s" s="9">
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>17</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>18</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>19</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>20</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>21</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>22</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>23</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>24</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>27</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>28</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>29</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>30</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>31</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>